<commit_message>
Update for new battery: Turnigy 5000 mAh 6S 25C LiPo
</commit_message>
<xml_diff>
--- a/PROPELLER_ShortFlight.xlsx
+++ b/PROPELLER_ShortFlight.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\AAE451\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\AAE451\Git\AAE451_Team7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC96AF0-A8DA-4597-8E53-299E7C943C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71096E31-2F8B-4E0D-A5D8-8A1BDD814975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2245,94 +2245,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>356.94947054920414</c:v>
+                  <c:v>461.86594938338646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>201.19634301594294</c:v>
+                  <c:v>260.14192660627987</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129.3220063809967</c:v>
+                  <c:v>166.95280257801909</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90.509502204663534</c:v>
+                  <c:v>116.52282015834662</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>67.346789947453814</c:v>
+                  <c:v>86.314421315315869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.560658318185737</c:v>
+                  <c:v>66.913406651569971</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.676482368844901</c:v>
+                  <c:v>53.82233882037626</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.864208726811675</c:v>
+                  <c:v>44.672458457004772</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.085566202661465</c:v>
+                  <c:v>38.119862350830395</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.715913820615885</c:v>
+                  <c:v>33.356036289586655</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25.361173641517386</c:v>
+                  <c:v>29.870899079588618</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.762763464725957</c:v>
+                  <c:v>27.329750641328971</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.745306502332966</c:v>
+                  <c:v>25.505589175335455</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.186454836346439</c:v>
+                  <c:v>24.240051662892494</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.998750222227123</c:v>
+                  <c:v>23.419935101904766</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.118331698473732</c:v>
+                  <c:v>22.962580017594068</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22.497688128253849</c:v>
+                  <c:v>22.806489596815727</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.100880707952925</c:v>
+                  <c:v>22.905145864251196</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.900318237983765</c:v>
+                  <c:v>23.222835701701761</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.874534067427874</c:v>
+                  <c:v>23.731773400207601</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26.006624280313879</c:v>
+                  <c:v>24.410079101040605</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.283131532953977</c:v>
+                  <c:v>25.240334072396664</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28.693234922919878</c:v>
+                  <c:v>26.208532103120771</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>30.228153619741853</c:v>
+                  <c:v>27.303307582397156</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31.880702144716107</c:v>
+                  <c:v>28.515359868930698</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>33.644954777631497</c:v>
+                  <c:v>29.837018910332247</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35.515989526333946</c:v>
+                  <c:v>31.261913845957768</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>37.489690809645751</c:v>
+                  <c:v>32.784717606333871</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39.562595955279555</c:v>
+                  <c:v>34.400948225234636</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41.731774736286624</c:v>
+                  <c:v>36.106812915723125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2357,10 +2357,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17.124025370746189</c:v>
+                  <c:v>19.133888134583913</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.124025370746189</c:v>
+                  <c:v>19.133888134583913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2407,10 +2407,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17.082217963388665</c:v>
+                  <c:v>19.087173752990996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.082217963388665</c:v>
+                  <c:v>19.087173752990996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2683,94 +2683,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>1070.8484116476125</c:v>
+                  <c:v>1385.5978481501593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>804.78537206377177</c:v>
+                  <c:v>1040.5677064251195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>646.61003190498354</c:v>
+                  <c:v>834.7640128900955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>543.0570132279812</c:v>
+                  <c:v>699.13692095007968</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>471.42752963217669</c:v>
+                  <c:v>604.20094920721112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>420.4852665454859</c:v>
+                  <c:v>535.30725321255977</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>384.08834131960413</c:v>
+                  <c:v>484.40104938338635</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>358.64208726811677</c:v>
+                  <c:v>446.72458457004774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>341.94122822927613</c:v>
+                  <c:v>419.31848585913434</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>332.59096584739063</c:v>
+                  <c:v>400.27243547503986</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>329.69525733972603</c:v>
+                  <c:v>388.32168803465203</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>332.67868850616338</c:v>
+                  <c:v>382.61650897860557</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>341.17959753499451</c:v>
+                  <c:v>382.58383763003184</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>354.98327738154302</c:v>
+                  <c:v>387.8408266062799</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>373.97875377786107</c:v>
+                  <c:v>398.138896732381</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>398.12997057252716</c:v>
+                  <c:v>413.32644031669321</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>427.45607443682314</c:v>
+                  <c:v>433.32330233949881</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>462.0176141590585</c:v>
+                  <c:v>458.10291728502392</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>501.90668299765906</c:v>
+                  <c:v>487.679549735737</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>547.23974948341322</c:v>
+                  <c:v>522.09901480456722</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>598.15235844721917</c:v>
+                  <c:v>561.43181932393395</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>654.79515679089548</c:v>
+                  <c:v>605.76801773751993</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>717.33087307299695</c:v>
+                  <c:v>655.21330257801924</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>785.93199411328817</c:v>
+                  <c:v>709.88599714232612</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>860.77895790733487</c:v>
+                  <c:v>769.91471646112882</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>942.05873377368198</c:v>
+                  <c:v>835.43652948930298</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1029.9636962636844</c:v>
+                  <c:v>906.5955015327753</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1124.6907242893726</c:v>
+                  <c:v>983.54152819001615</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1226.4404746136663</c:v>
+                  <c:v>1066.4293949822736</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1335.416791561172</c:v>
+                  <c:v>1155.41801330314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2795,10 +2795,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17.124025370746189</c:v>
+                  <c:v>19.133888134583913</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.124025370746189</c:v>
+                  <c:v>19.133888134583913</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2845,10 +2845,10 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>17.082217963388665</c:v>
+                  <c:v>19.087173752990996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.082217963388665</c:v>
+                  <c:v>19.087173752990996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3183,97 +3183,97 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1652701142105765</c:v>
+                  <c:v>0.13238197049685027</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37157416089154005</c:v>
+                  <c:v>0.29771365519275511</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65922271752966244</c:v>
+                  <c:v>0.52857223667797903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0256042549266378</c:v>
+                  <c:v>0.82360881564562416</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4654063581090611</c:v>
+                  <c:v>1.1800589774015224</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.969406412740456</c:v>
+                  <c:v>1.5930570802031314</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5234311031091017</c:v>
+                  <c:v>2.0549514197656502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1078756410539166</c:v>
+                  <c:v>2.5547719220990692</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6982051105687699</c:v>
+                  <c:v>3.0780441629900719</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2667133400531183</c:v>
+                  <c:v>3.607143140615372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7854528939018302</c:v>
+                  <c:v>4.1223063437824301</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2297737429183284</c:v>
+                  <c:v>4.6032695445032354</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5815562107026855</c:v>
+                  <c:v>5.0312863005805157</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8312337970207588</c:v>
+                  <c:v>5.3911242377011872</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.9781159711337377</c:v>
+                  <c:v>5.6725869198742505</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.0291243211621142</c:v>
+                  <c:v>5.8712289082652793</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.9965282105409576</c:v>
+                  <c:v>5.9881685722877727</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.8954146418907758</c:v>
+                  <c:v>6.0291523347459179</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.7414780707619721</c:v>
+                  <c:v>6.0031837742891936</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5494323832563737</c:v>
+                  <c:v>5.9210598467061351</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.3320878148096638</c:v>
+                  <c:v>5.7940802687251836</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.0999775507349794</c:v>
+                  <c:v>5.6330747405950934</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.8613627742768015</c:v>
+                  <c:v>5.4477805089900508</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.6224554448565822</c:v>
+                  <c:v>5.2465280947049608</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.3877373943666198</c:v>
+                  <c:v>5.0361590655284099</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.1602973296490768</c:v>
+                  <c:v>4.8220959031212915</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.9421423175215513</c:v>
+                  <c:v>4.6084965932164188</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.7344644417595863</c:v>
+                  <c:v>4.3984447234275628</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.537857932023134</c:v>
+                  <c:v>4.1941431874171409</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.3524898151255003</c:v>
+                  <c:v>3.9970933097458876</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.1782305171093705</c:v>
+                  <c:v>3.8082508229388035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24833,8 +24833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24973,7 +24973,8 @@
         <v>25</v>
       </c>
       <c r="C17" s="59">
-        <v>60904.879849999998</v>
+        <f>5000*3.6*22.2/C26</f>
+        <v>62189.228937600667</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -24985,7 +24986,7 @@
       </c>
       <c r="C19" s="32">
         <f>(C6*C10/C14+C14/(C6*PI()*C8*C9))*C7/C17</f>
-        <v>5.4761838955495711E-2</v>
+        <v>5.3630882371866147E-2</v>
       </c>
       <c r="R19" s="32"/>
     </row>
@@ -25022,22 +25023,22 @@
         <v>31</v>
       </c>
       <c r="C25" s="1">
-        <f>(11.72+1.814)*9.8</f>
-        <v>132.63320000000002</v>
+        <f>14.031*9.8</f>
+        <v>137.50380000000001</v>
       </c>
       <c r="D25" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1">
         <f>C25/9.80665</f>
-        <v>13.524822441914418</v>
+        <v>14.021485420607448</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="1">
         <f>0.224809*C25</f>
-        <v>29.817137058800004</v>
+        <v>30.912091774200004</v>
       </c>
       <c r="H25" t="s">
         <v>32</v>
@@ -25048,18 +25049,19 @@
         <v>33</v>
       </c>
       <c r="C26" s="1">
-        <v>11.66</v>
+        <f>0.655*9.81</f>
+        <v>6.4255500000000003</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="1">
         <f>C26/9.80665</f>
-        <v>1.1889891043322645</v>
+        <v>0.65522375123003274</v>
       </c>
       <c r="G26" s="1">
         <f>0.224809*C26</f>
-        <v>2.6212729400000003</v>
+        <v>1.4445214699500002</v>
       </c>
       <c r="H26" t="s">
         <v>32</v>
@@ -25075,7 +25077,7 @@
       </c>
       <c r="C28" s="1">
         <f>C15*C25</f>
-        <v>1193.6988000000001</v>
+        <v>1237.5342000000001</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
@@ -25096,7 +25098,7 @@
       </c>
       <c r="C29" s="1">
         <f>C28/C5</f>
-        <v>66.316600000000008</v>
+        <v>68.751900000000006</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -25106,7 +25108,7 @@
       </c>
       <c r="G29">
         <f>C28*G28</f>
-        <v>290068.80840000004</v>
+        <v>300720.81060000003</v>
       </c>
       <c r="H29" t="s">
         <v>46</v>
@@ -25126,8 +25128,7 @@
         <v>37</v>
       </c>
       <c r="C31" s="1">
-        <f>C25/C14</f>
-        <v>0.61539389502040831</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -25139,7 +25140,7 @@
       </c>
       <c r="C32" s="1">
         <f>SQRT(C8*C31)</f>
-        <v>1.7790364813825374</v>
+        <v>1.6211332456032108</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
@@ -25151,7 +25152,7 @@
       </c>
       <c r="C33" s="1">
         <f>C31/C32</f>
-        <v>0.34591415154239502</v>
+        <v>0.31521159743402893</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
@@ -25163,14 +25164,14 @@
       </c>
       <c r="C35" s="2">
         <f>C25/(C6*C31)</f>
-        <v>1.0860453514739228</v>
+        <v>1.3559469449880408</v>
       </c>
       <c r="E35" t="s">
         <v>183</v>
       </c>
       <c r="F35">
         <f>C35*C6*C31</f>
-        <v>132.63320000000002</v>
+        <v>137.50380000000001</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -25179,7 +25180,7 @@
       </c>
       <c r="C36" s="2">
         <f>C29/(C6*C31)</f>
-        <v>0.54302267573696139</v>
+        <v>0.6779734724940204</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -25264,14 +25265,14 @@
       </c>
       <c r="C3" s="1">
         <f>'weight analysis'!C25</f>
-        <v>132.63320000000002</v>
+        <v>137.50380000000001</v>
       </c>
       <c r="Q3" t="s">
         <v>126</v>
       </c>
       <c r="R3" s="1">
         <f>SQRT(2*C3/(C5*C4*R2))</f>
-        <v>17.082217963388665</v>
+        <v>19.087173752990996</v>
       </c>
       <c r="S3" t="s">
         <v>1</v>
@@ -25283,7 +25284,7 @@
       </c>
       <c r="C4" s="1">
         <f>'weight analysis'!C31</f>
-        <v>0.61539389502040831</v>
+        <v>0.51100000000000001</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
@@ -25302,7 +25303,7 @@
       </c>
       <c r="R5" s="1">
         <f>SQRT(2*C6/(C5*C4*C2))</f>
-        <v>17.124025370746189</v>
+        <v>19.133888134583913</v>
       </c>
       <c r="S5" t="s">
         <v>1</v>
@@ -25314,7 +25315,7 @@
       </c>
       <c r="C6" s="1">
         <f>'weight analysis'!C25</f>
-        <v>132.63320000000002</v>
+        <v>137.50380000000001</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -25351,7 +25352,7 @@
       </c>
       <c r="G8" s="1">
         <f>R5</f>
-        <v>17.124025370746189</v>
+        <v>19.133888134583913</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -25361,7 +25362,7 @@
       </c>
       <c r="K8" s="1">
         <f>R3</f>
-        <v>17.082217963388665</v>
+        <v>19.087173752990996</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
@@ -25374,7 +25375,7 @@
       </c>
       <c r="G9" s="1">
         <f>R5</f>
-        <v>17.124025370746189</v>
+        <v>19.133888134583913</v>
       </c>
       <c r="H9">
         <v>30</v>
@@ -25384,7 +25385,7 @@
       </c>
       <c r="K9" s="1">
         <f>R3</f>
-        <v>17.082217963388665</v>
+        <v>19.087173752990996</v>
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
@@ -25393,7 +25394,7 @@
       </c>
       <c r="C10" s="1">
         <f>'weight analysis'!C31</f>
-        <v>0.61539389502040831</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -25452,23 +25453,23 @@
       </c>
       <c r="I12">
         <f t="shared" ref="I12:I44" si="2">$C$6/(H12*$C$10)</f>
-        <v>87.969673469387743</v>
+        <v>109.83170254403132</v>
       </c>
       <c r="J12">
         <f t="shared" ref="J12:J44" si="3">H12*$C$10*($C$9+I12^2/(PI()*$C$7*$C$8))</f>
-        <v>802.52379949957174</v>
+        <v>1038.6897814251195</v>
       </c>
       <c r="K12">
         <f t="shared" ref="K12:K44" si="4">J12*G12</f>
-        <v>1605.0475989991435</v>
+        <v>2077.3795628502389</v>
       </c>
       <c r="L12">
         <f>J12/(1/2*1.225*G12^2*$C$10)</f>
-        <v>532.27816710589593</v>
+        <v>829.65755934751337</v>
       </c>
       <c r="M12">
         <f>I12/L12</f>
-        <v>0.1652701142105765</v>
+        <v>0.13238197049685027</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
@@ -25494,23 +25495,23 @@
       </c>
       <c r="I13">
         <f t="shared" si="2"/>
-        <v>39.097632653061225</v>
+        <v>48.814090019569477</v>
       </c>
       <c r="J13">
         <f t="shared" si="3"/>
-        <v>356.94947054920414</v>
+        <v>461.86594938338646</v>
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>1070.8484116476125</v>
+        <v>1385.5978481501593</v>
       </c>
       <c r="L13">
         <f t="shared" ref="L13:L44" si="8">J13/(1/2*1.225*G13^2*$C$10)</f>
-        <v>105.22161325548564</v>
+        <v>163.96322159950884</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:M44" si="9">I13/L13</f>
-        <v>0.37157416089154005</v>
+        <v>0.29771365519275511</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -25536,23 +25537,23 @@
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>21.992418367346936</v>
+        <v>27.457925636007829</v>
       </c>
       <c r="J14">
         <f t="shared" si="3"/>
-        <v>201.19634301594294</v>
+        <v>260.14192660627987</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>804.78537206377177</v>
+        <v>1040.5677064251195</v>
       </c>
       <c r="L14">
         <f t="shared" si="8"/>
-        <v>33.361135444118496</v>
+        <v>51.947347459219586</v>
       </c>
       <c r="M14">
         <f t="shared" si="9"/>
-        <v>0.65922271752966244</v>
+        <v>0.52857223667797903</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
@@ -25578,23 +25579,23 @@
       </c>
       <c r="I15">
         <f t="shared" si="2"/>
-        <v>14.075147755102041</v>
+        <v>17.573072407045007</v>
       </c>
       <c r="J15">
         <f t="shared" si="3"/>
-        <v>129.3220063809967</v>
+        <v>166.95280257801909</v>
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>646.61003190498354</v>
+        <v>834.7640128900955</v>
       </c>
       <c r="L15">
         <f t="shared" si="8"/>
-        <v>13.72376107791094</v>
+        <v>21.336673519296337</v>
       </c>
       <c r="M15">
         <f t="shared" si="9"/>
-        <v>1.0256042549266378</v>
+        <v>0.82360881564562416</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
@@ -25620,23 +25621,23 @@
       </c>
       <c r="I16">
         <f t="shared" si="2"/>
-        <v>9.7744081632653064</v>
+        <v>12.203522504892369</v>
       </c>
       <c r="J16">
         <f t="shared" si="3"/>
-        <v>90.509502204663534</v>
+        <v>116.52282015834662</v>
       </c>
       <c r="K16">
         <f t="shared" si="4"/>
-        <v>543.0570132279812</v>
+        <v>699.13692095007968</v>
       </c>
       <c r="L16">
         <f t="shared" si="8"/>
-        <v>6.6701008284678522</v>
+        <v>10.341451349969303</v>
       </c>
       <c r="M16">
         <f t="shared" si="9"/>
-        <v>1.4654063581090611</v>
+        <v>1.1800589774015224</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
@@ -25662,23 +25663,23 @@
       </c>
       <c r="I17">
         <f t="shared" si="2"/>
-        <v>7.1811978342357348</v>
+        <v>8.9658532689005153</v>
       </c>
       <c r="J17">
         <f t="shared" si="3"/>
-        <v>67.346789947453814</v>
+        <v>86.314421315315869</v>
       </c>
       <c r="K17">
         <f t="shared" si="4"/>
-        <v>471.42752963217669</v>
+        <v>604.20094920721112</v>
       </c>
       <c r="L17">
         <f t="shared" si="8"/>
-        <v>3.6463767903766495</v>
+        <v>5.6280803621658526</v>
       </c>
       <c r="M17">
         <f t="shared" si="9"/>
-        <v>1.969406412740456</v>
+        <v>1.5930570802031314</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
@@ -25704,23 +25705,23 @@
       </c>
       <c r="I18">
         <f t="shared" si="2"/>
-        <v>5.4981045918367339</v>
+        <v>6.8644814090019572</v>
       </c>
       <c r="J18">
         <f t="shared" si="3"/>
-        <v>52.560658318185737</v>
+        <v>66.913406651569971</v>
       </c>
       <c r="K18">
         <f t="shared" si="4"/>
-        <v>420.4852665454859</v>
+        <v>535.30725321255977</v>
       </c>
       <c r="L18">
         <f t="shared" si="8"/>
-        <v>2.178820965257406</v>
+        <v>3.3404592162012245</v>
       </c>
       <c r="M18">
         <f t="shared" si="9"/>
-        <v>2.5234311031091017</v>
+        <v>2.0549514197656502</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -25746,23 +25747,23 @@
       </c>
       <c r="I19">
         <f t="shared" si="2"/>
-        <v>4.3441814058956911</v>
+        <v>5.4237877799521632</v>
       </c>
       <c r="J19">
         <f t="shared" si="3"/>
-        <v>42.676482368844901</v>
+        <v>53.82233882037626</v>
       </c>
       <c r="K19">
         <f t="shared" si="4"/>
-        <v>384.08834131960413</v>
+        <v>484.40104938338635</v>
       </c>
       <c r="L19">
         <f t="shared" si="8"/>
-        <v>1.3977976945121682</v>
+        <v>2.1230027357964047</v>
       </c>
       <c r="M19">
         <f t="shared" si="9"/>
-        <v>3.1078756410539166</v>
+        <v>2.5547719220990692</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
@@ -25788,23 +25789,23 @@
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>3.5187869387755102</v>
+        <v>4.3932681017612518</v>
       </c>
       <c r="J20">
         <f t="shared" si="3"/>
-        <v>35.864208726811675</v>
+        <v>44.672458457004772</v>
       </c>
       <c r="K20">
         <f t="shared" si="4"/>
-        <v>358.64208726811677</v>
+        <v>446.72458457004774</v>
       </c>
       <c r="L20">
         <f t="shared" si="8"/>
-        <v>0.95148506736943372</v>
+        <v>1.4272920949560211</v>
       </c>
       <c r="M20">
         <f t="shared" si="9"/>
-        <v>3.6982051105687699</v>
+        <v>3.0780441629900719</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -25830,23 +25831,23 @@
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>2.9080883791533139</v>
+        <v>3.6308000841002084</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>31.085566202661465</v>
+        <v>38.119862350830395</v>
       </c>
       <c r="K21">
         <f t="shared" si="4"/>
-        <v>341.94122822927613</v>
+        <v>419.31848585913434</v>
       </c>
       <c r="L21">
         <f t="shared" si="8"/>
-        <v>0.68157575805575676</v>
+        <v>1.0065583600546555</v>
       </c>
       <c r="M21">
         <f t="shared" si="9"/>
-        <v>4.2667133400531183</v>
+        <v>3.607143140615372</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -25872,23 +25873,23 @@
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>2.4436020408163266</v>
+        <v>3.0508806262230923</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>27.715913820615885</v>
+        <v>33.356036289586655</v>
       </c>
       <c r="K22">
         <f t="shared" si="4"/>
-        <v>332.59096584739063</v>
+        <v>400.27243547503986</v>
       </c>
       <c r="L22">
         <f t="shared" si="8"/>
-        <v>0.51063130177924076</v>
+        <v>0.74009070937308141</v>
       </c>
       <c r="M22">
         <f t="shared" si="9"/>
-        <v>4.7854528939018302</v>
+        <v>4.1223063437824301</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -25914,23 +25915,23 @@
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>2.0821224489795918</v>
+        <v>2.5995669241190842</v>
       </c>
       <c r="J23">
         <f t="shared" si="3"/>
-        <v>25.361173641517386</v>
+        <v>29.870899079588618</v>
       </c>
       <c r="K23">
         <f t="shared" si="4"/>
-        <v>329.69525733972603</v>
+        <v>388.32168803465203</v>
       </c>
       <c r="L23">
         <f t="shared" si="8"/>
-        <v>0.39812859051483973</v>
+        <v>0.56472185671230735</v>
       </c>
       <c r="M23">
         <f t="shared" si="9"/>
-        <v>5.2297737429183284</v>
+        <v>4.6032695445032354</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
@@ -25956,23 +25957,23 @@
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>1.7952994585589337</v>
+        <v>2.2414633172251288</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>23.762763464725957</v>
+        <v>27.329750641328971</v>
       </c>
       <c r="K24">
         <f t="shared" si="4"/>
-        <v>332.67868850616338</v>
+        <v>382.61650897860557</v>
       </c>
       <c r="L24">
         <f t="shared" si="8"/>
-        <v>0.3216485493985406</v>
+        <v>0.44550502263536584</v>
       </c>
       <c r="M24">
         <f t="shared" si="9"/>
-        <v>5.5815562107026855</v>
+        <v>5.0312863005805157</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
@@ -25998,23 +25999,23 @@
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>1.5639053061224488</v>
+        <v>1.9525636007827789</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>22.745306502332966</v>
+        <v>25.505589175335455</v>
       </c>
       <c r="K25">
         <f t="shared" si="4"/>
-        <v>341.17959753499451</v>
+        <v>382.58383763003184</v>
       </c>
       <c r="L25">
         <f t="shared" si="8"/>
-        <v>0.26819458120877698</v>
+        <v>0.36218115455921407</v>
       </c>
       <c r="M25">
         <f t="shared" si="9"/>
-        <v>5.8312337970207588</v>
+        <v>5.3911242377011872</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -26040,23 +26041,23 @@
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>1.3745261479591835</v>
+        <v>1.7161203522504893</v>
       </c>
       <c r="J26">
         <f t="shared" si="3"/>
-        <v>22.186454836346439</v>
+        <v>24.240051662892494</v>
       </c>
       <c r="K26">
         <f t="shared" si="4"/>
-        <v>354.98327738154302</v>
+        <v>387.8408266062799</v>
       </c>
       <c r="L26">
         <f t="shared" si="8"/>
-        <v>0.2299263103285879</v>
+        <v>0.30252870101257651</v>
       </c>
       <c r="M26">
         <f t="shared" si="9"/>
-        <v>5.9781159711337377</v>
+        <v>5.6725869198742505</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
@@ -26082,23 +26083,23 @@
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>1.2175733352164393</v>
+        <v>1.5201619729277691</v>
       </c>
       <c r="J27">
         <f t="shared" si="3"/>
-        <v>21.998750222227123</v>
+        <v>23.419935101904766</v>
       </c>
       <c r="K27">
         <f t="shared" si="4"/>
-        <v>373.97875377786107</v>
+        <v>398.138896732381</v>
       </c>
       <c r="L27">
         <f t="shared" si="8"/>
-        <v>0.20194861979255918</v>
+        <v>0.25891716992804459</v>
       </c>
       <c r="M27">
         <f t="shared" si="9"/>
-        <v>6.0291243211621142</v>
+        <v>5.8712289082652793</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -26124,23 +26125,23 @@
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>1.0860453514739228</v>
+        <v>1.3559469449880408</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
-        <v>22.118331698473732</v>
+        <v>22.962580017594068</v>
       </c>
       <c r="K28">
         <f t="shared" si="4"/>
-        <v>398.12997057252716</v>
+        <v>413.32644031669321</v>
       </c>
       <c r="L28">
         <f t="shared" si="8"/>
-        <v>0.18111235590701052</v>
+        <v>0.2264376709872753</v>
       </c>
       <c r="M28">
         <f t="shared" si="9"/>
-        <v>5.9965282105409576</v>
+        <v>5.9881685722877727</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
@@ -26166,23 +26167,23 @@
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
-        <v>0.97473322403753748</v>
+        <v>1.2169717733410672</v>
       </c>
       <c r="J29">
         <f t="shared" si="3"/>
-        <v>22.497688128253849</v>
+        <v>22.806489596815727</v>
       </c>
       <c r="K29">
         <f t="shared" si="4"/>
-        <v>427.45607443682314</v>
+        <v>433.32330233949881</v>
       </c>
       <c r="L29">
         <f t="shared" si="8"/>
-        <v>0.16533751792646112</v>
+        <v>0.20184790593657362</v>
       </c>
       <c r="M29">
         <f t="shared" si="9"/>
-        <v>5.8954146418907758</v>
+        <v>6.0291523347459179</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
@@ -26208,23 +26209,23 @@
       </c>
       <c r="I30">
         <f t="shared" si="2"/>
-        <v>0.87969673469387755</v>
+        <v>1.098317025440313</v>
       </c>
       <c r="J30">
         <f t="shared" si="3"/>
-        <v>23.100880707952925</v>
+        <v>22.905145864251196</v>
       </c>
       <c r="K30">
         <f t="shared" si="4"/>
-        <v>462.0176141590585</v>
+        <v>458.10291728502392</v>
       </c>
       <c r="L30">
         <f t="shared" si="8"/>
-        <v>0.15321781671058962</v>
+        <v>0.18295575593475133</v>
       </c>
       <c r="M30">
         <f t="shared" si="9"/>
-        <v>5.7414780707619721</v>
+        <v>6.0031837742891936</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
@@ -26250,23 +26251,23 @@
       </c>
       <c r="I31">
         <f t="shared" si="2"/>
-        <v>0.79791087047063713</v>
+        <v>0.99620591876672393</v>
       </c>
       <c r="J31">
         <f t="shared" si="3"/>
-        <v>23.900318237983765</v>
+        <v>23.222835701701761</v>
       </c>
       <c r="K31">
         <f t="shared" si="4"/>
-        <v>501.90668299765906</v>
+        <v>487.679549735737</v>
       </c>
       <c r="L31">
         <f t="shared" si="8"/>
-        <v>0.14378242951082285</v>
+        <v>0.16824790570575127</v>
       </c>
       <c r="M31">
         <f t="shared" si="9"/>
-        <v>5.5494323832563737</v>
+        <v>5.9210598467061351</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
@@ -26292,23 +26293,23 @@
       </c>
       <c r="I32">
         <f t="shared" si="2"/>
-        <v>0.72702209478832847</v>
+        <v>0.9077000210250521</v>
       </c>
       <c r="J32">
         <f t="shared" si="3"/>
-        <v>24.874534067427874</v>
+        <v>23.731773400207601</v>
       </c>
       <c r="K32">
         <f t="shared" si="4"/>
-        <v>547.23974948341322</v>
+        <v>522.09901480456722</v>
       </c>
       <c r="L32">
         <f t="shared" si="8"/>
-        <v>0.1363484848784848</v>
+        <v>0.15665989750341597</v>
       </c>
       <c r="M32">
         <f t="shared" si="9"/>
-        <v>5.3320878148096638</v>
+        <v>5.7940802687251836</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
@@ -26334,23 +26335,23 @@
       </c>
       <c r="I33">
         <f t="shared" si="2"/>
-        <v>0.66517711508043664</v>
+        <v>0.8304854634709361</v>
       </c>
       <c r="J33">
         <f t="shared" si="3"/>
-        <v>26.006624280313879</v>
+        <v>24.410079101040605</v>
       </c>
       <c r="K33">
         <f t="shared" si="4"/>
-        <v>598.15235844721917</v>
+        <v>561.43181932393395</v>
       </c>
       <c r="L33">
         <f t="shared" si="8"/>
-        <v>0.13042745942765477</v>
+        <v>0.14743022269631759</v>
       </c>
       <c r="M33">
         <f t="shared" si="9"/>
-        <v>5.0999775507349794</v>
+        <v>5.6330747405950934</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
@@ -26376,23 +26377,23 @@
       </c>
       <c r="I34">
         <f t="shared" si="2"/>
-        <v>0.61090051020408165</v>
+        <v>0.76272015655577308</v>
       </c>
       <c r="J34">
         <f t="shared" si="3"/>
-        <v>27.283131532953977</v>
+        <v>25.240334072396664</v>
       </c>
       <c r="K34">
         <f t="shared" si="4"/>
-        <v>654.79515679089548</v>
+        <v>605.76801773751993</v>
       </c>
       <c r="L34">
         <f t="shared" si="8"/>
-        <v>0.12566445636120255</v>
+        <v>0.1400056693358176</v>
       </c>
       <c r="M34">
         <f t="shared" si="9"/>
-        <v>4.8613627742768015</v>
+        <v>5.4477805089900508</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -26418,23 +26419,23 @@
       </c>
       <c r="I35">
         <f t="shared" si="2"/>
-        <v>0.56300591020408164</v>
+        <v>0.70292289628180049</v>
       </c>
       <c r="J35">
         <f t="shared" si="3"/>
-        <v>28.693234922919878</v>
+        <v>26.208532103120771</v>
       </c>
       <c r="K35">
         <f t="shared" si="4"/>
-        <v>717.33087307299695</v>
+        <v>655.21330257801924</v>
       </c>
       <c r="L35">
         <f t="shared" si="8"/>
-        <v>0.12179801772465751</v>
+        <v>0.13397867763087418</v>
       </c>
       <c r="M35">
         <f t="shared" si="9"/>
-        <v>4.6224554448565822</v>
+        <v>5.2465280947049608</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
@@ -26460,23 +26461,23 @@
       </c>
       <c r="I36">
         <f t="shared" si="2"/>
-        <v>0.52053061224489794</v>
+        <v>0.64989173102977105</v>
       </c>
       <c r="J36">
         <f t="shared" si="3"/>
-        <v>30.228153619741853</v>
+        <v>27.303307582397156</v>
       </c>
       <c r="K36">
         <f t="shared" si="4"/>
-        <v>785.93199411328817</v>
+        <v>709.88599714232612</v>
       </c>
       <c r="L36">
         <f t="shared" si="8"/>
-        <v>0.11863303690717748</v>
+        <v>0.12904511604451921</v>
       </c>
       <c r="M36">
         <f t="shared" si="9"/>
-        <v>4.3877373943666198</v>
+        <v>5.0361590655284099</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
@@ -26490,23 +26491,23 @@
       </c>
       <c r="I37">
         <f t="shared" si="2"/>
-        <v>0.48268682287729908</v>
+        <v>0.60264308666135147</v>
       </c>
       <c r="J37">
         <f t="shared" si="3"/>
-        <v>31.880702144716107</v>
+        <v>28.515359868930698</v>
       </c>
       <c r="K37">
         <f t="shared" si="4"/>
-        <v>860.77895790733487</v>
+        <v>769.91471646112882</v>
       </c>
       <c r="L37">
         <f t="shared" si="8"/>
-        <v>0.11602219375940949</v>
+        <v>0.12497534241723957</v>
       </c>
       <c r="M37">
         <f t="shared" si="9"/>
-        <v>4.1602973296490768</v>
+        <v>4.8220959031212915</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
@@ -26520,23 +26521,23 @@
       </c>
       <c r="I38">
         <f t="shared" si="2"/>
-        <v>0.44882486463973342</v>
+        <v>0.5603658293062822</v>
       </c>
       <c r="J38">
         <f t="shared" si="3"/>
-        <v>33.644954777631497</v>
+        <v>29.837018910332247</v>
       </c>
       <c r="K38">
         <f t="shared" si="4"/>
-        <v>942.05873377368198</v>
+        <v>835.43652948930298</v>
       </c>
       <c r="L38">
         <f t="shared" si="8"/>
-        <v>0.11385303433740879</v>
+        <v>0.12159406391471037</v>
       </c>
       <c r="M38">
         <f t="shared" si="9"/>
-        <v>3.9421423175215513</v>
+        <v>4.6084965932164188</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
@@ -26550,23 +26551,23 @@
       </c>
       <c r="I39">
         <f t="shared" si="2"/>
-        <v>0.41840510568079786</v>
+        <v>0.52238621899658166</v>
       </c>
       <c r="J39">
         <f t="shared" si="3"/>
-        <v>35.515989526333946</v>
+        <v>31.261913845957768</v>
       </c>
       <c r="K39">
         <f t="shared" si="4"/>
-        <v>1029.9636962636844</v>
+        <v>906.5955015327753</v>
       </c>
       <c r="L39">
         <f t="shared" si="8"/>
-        <v>0.11203885114076916</v>
+        <v>0.11876612117328221</v>
       </c>
       <c r="M39">
         <f t="shared" si="9"/>
-        <v>3.7344644417595863</v>
+        <v>4.3984447234275628</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
@@ -26580,23 +26581,23 @@
       </c>
       <c r="I40">
         <f t="shared" si="2"/>
-        <v>0.39097632653061221</v>
+        <v>0.48814090019569473</v>
       </c>
       <c r="J40">
         <f t="shared" si="3"/>
-        <v>37.489690809645751</v>
+        <v>32.784717606333871</v>
       </c>
       <c r="K40">
         <f t="shared" si="4"/>
-        <v>1124.6907242893726</v>
+        <v>983.54152819001615</v>
       </c>
       <c r="L40">
         <f t="shared" si="8"/>
-        <v>0.11051216132554856</v>
+        <v>0.1163863221599509</v>
       </c>
       <c r="M40">
         <f t="shared" si="9"/>
-        <v>3.537857932023134</v>
+        <v>4.1941431874171409</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
@@ -26610,23 +26611,23 @@
       </c>
       <c r="I41">
         <f t="shared" si="2"/>
-        <v>0.36615889061139539</v>
+        <v>0.45715588988150391</v>
       </c>
       <c r="J41">
         <f t="shared" si="3"/>
-        <v>39.562595955279555</v>
+        <v>34.400948225234636</v>
       </c>
       <c r="K41">
         <f t="shared" si="4"/>
-        <v>1226.4404746136663</v>
+        <v>1066.4293949822736</v>
       </c>
       <c r="L41">
         <f t="shared" si="8"/>
-        <v>0.10921998598157956</v>
+        <v>0.11437208352550751</v>
       </c>
       <c r="M41">
         <f t="shared" si="9"/>
-        <v>3.3524898151255003</v>
+        <v>3.9970933097458876</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
@@ -26640,23 +26641,23 @@
       </c>
       <c r="I42">
         <f t="shared" si="2"/>
-        <v>0.34363153698979587</v>
+        <v>0.42903008806262233</v>
       </c>
       <c r="J42">
         <f t="shared" si="3"/>
-        <v>41.731774736286624</v>
+        <v>36.106812915723125</v>
       </c>
       <c r="K42">
         <f t="shared" si="4"/>
-        <v>1335.416791561172</v>
+        <v>1155.41801330314</v>
       </c>
       <c r="L42">
         <f t="shared" si="8"/>
-        <v>0.10812039439553675</v>
+        <v>0.11265804381328604</v>
       </c>
       <c r="M42">
         <f t="shared" si="9"/>
-        <v>3.1782305171093705</v>
+        <v>3.8082508229388035</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
@@ -26669,23 +26670,23 @@
       </c>
       <c r="I43">
         <f t="shared" si="2"/>
-        <v>3.9570322134469764</v>
+        <v>4.9404251247527444</v>
       </c>
       <c r="J43">
         <f t="shared" si="3"/>
-        <v>39.443999656913952</v>
+        <v>49.499718588893458</v>
       </c>
       <c r="K43">
         <f t="shared" si="4"/>
-        <v>371.95691676469858</v>
+        <v>466.78234629326528</v>
       </c>
       <c r="L43">
         <f t="shared" si="8"/>
-        <v>1.1767881440664929</v>
+        <v>1.778493782606442</v>
       </c>
       <c r="M43">
         <f t="shared" si="9"/>
-        <v>3.3625697483432408</v>
+        <v>2.7778703378498104</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
@@ -26698,23 +26699,23 @@
       </c>
       <c r="I44">
         <f t="shared" si="2"/>
-        <v>4.746644083703969</v>
+        <v>5.9262695940911589</v>
       </c>
       <c r="J44">
         <f t="shared" si="3"/>
-        <v>46.08848103558509</v>
+        <v>58.358831902482152</v>
       </c>
       <c r="K44">
         <f t="shared" si="4"/>
-        <v>396.8218217163876</v>
+        <v>502.46954268037132</v>
       </c>
       <c r="L44">
         <f t="shared" si="8"/>
-        <v>1.64940313461835</v>
+        <v>2.515204460170243</v>
       </c>
       <c r="M44">
         <f t="shared" si="9"/>
-        <v>2.8777949938856393</v>
+        <v>2.3561780713803424</v>
       </c>
     </row>
   </sheetData>
@@ -26814,7 +26815,7 @@
       </c>
       <c r="C7" s="26">
         <f>'weight analysis'!C31</f>
-        <v>0.61539389502040831</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="D7" t="str">
         <f>'weight analysis'!D31</f>
@@ -26828,7 +26829,7 @@
       </c>
       <c r="C8" s="26">
         <f>'weight analysis'!C32</f>
-        <v>1.7790364813825374</v>
+        <v>1.6211332456032108</v>
       </c>
       <c r="D8" t="str">
         <f>'weight analysis'!D32</f>
@@ -26842,7 +26843,7 @@
       </c>
       <c r="C9" s="26">
         <f>'weight analysis'!C33</f>
-        <v>0.34591415154239502</v>
+        <v>0.31521159743402893</v>
       </c>
       <c r="D9" t="str">
         <f>'weight analysis'!D33</f>
@@ -26906,7 +26907,7 @@
       </c>
       <c r="C17" s="11">
         <f>0.4*C8</f>
-        <v>0.71161459255301507</v>
+        <v>0.64845329824128439</v>
       </c>
       <c r="D17" t="s">
         <v>39</v>
@@ -26922,7 +26923,7 @@
       </c>
       <c r="K17" s="11">
         <f>0.4*C8</f>
-        <v>0.71161459255301507</v>
+        <v>0.64845329824128439</v>
       </c>
       <c r="L17" t="s">
         <v>39</v>
@@ -26940,7 +26941,7 @@
       </c>
       <c r="C18" s="11">
         <f>C16*C7*C9/C17</f>
-        <v>0.2093990504152663</v>
+        <v>0.1738771145245965</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -26950,7 +26951,7 @@
       </c>
       <c r="K18" s="11">
         <f>K16*C7*C8/K17</f>
-        <v>7.6924236877551039E-2</v>
+        <v>6.3875000000000001E-2</v>
       </c>
       <c r="L18" t="s">
         <v>11</v>
@@ -26988,7 +26989,7 @@
       </c>
       <c r="C20" s="11">
         <f>SQRT(C18/C19)</f>
-        <v>0.22880070498977179</v>
+        <v>0.20849287429346147</v>
       </c>
       <c r="D20" t="s">
         <v>39</v>
@@ -26998,7 +26999,7 @@
       </c>
       <c r="K20" s="11">
         <f>SQRT(K18/K19)</f>
-        <v>0.13867609462119906</v>
+        <v>0.12636751956100112</v>
       </c>
       <c r="L20" t="s">
         <v>39</v>
@@ -27010,7 +27011,7 @@
       </c>
       <c r="C21" s="11">
         <f>C18/C20</f>
-        <v>0.91520281995908703</v>
+        <v>0.83397149717384589</v>
       </c>
       <c r="D21" t="s">
         <v>39</v>
@@ -27020,7 +27021,7 @@
       </c>
       <c r="K21" s="11">
         <f>K18/K20</f>
-        <v>0.55470437848479637</v>
+        <v>0.50547007824400447</v>
       </c>
       <c r="L21" t="s">
         <v>39</v>
@@ -27359,7 +27360,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27418,7 +27419,7 @@
       </c>
       <c r="B8" s="62">
         <f>B6*'weight analysis'!C33/'weight analysis'!C3</f>
-        <v>484279.81215935299</v>
+        <v>441296.23640764045</v>
       </c>
       <c r="C8" s="19"/>
     </row>
@@ -27428,7 +27429,7 @@
       </c>
       <c r="B9" s="63">
         <f>'weight analysis'!C25/(B7*'weight analysis'!C31)</f>
-        <v>0.79791087047063713</v>
+        <v>0.99620591876672393</v>
       </c>
       <c r="C9" s="19"/>
     </row>
@@ -27447,7 +27448,7 @@
       </c>
       <c r="B11" s="63">
         <f>B9^2/(PI()*B10*'weight analysis'!C8)</f>
-        <v>4.3782429510822833E-2</v>
+        <v>6.8247905705751274E-2</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>104</v>
@@ -27470,7 +27471,7 @@
       </c>
       <c r="B13" s="63">
         <f>B12+B11</f>
-        <v>8.6782429510822823E-2</v>
+        <v>0.11124790570575127</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>290</v>
@@ -27482,14 +27483,14 @@
       </c>
       <c r="B14" s="64">
         <f>B7*B13*'weight analysis'!C31</f>
-        <v>14.425459980267858</v>
+        <v>15.355268914201764</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D14">
         <f>B14/2</f>
-        <v>7.212729990133929</v>
+        <v>7.6776344571008819</v>
       </c>
       <c r="E14" t="s">
         <v>279</v>
@@ -27501,7 +27502,7 @@
       </c>
       <c r="B15" s="62">
         <f>'weight analysis'!C25/B14</f>
-        <v>9.194382722036238</v>
+        <v>8.9548285196637387</v>
       </c>
       <c r="C15" s="19"/>
     </row>
@@ -27511,7 +27512,7 @@
       </c>
       <c r="B16" s="20">
         <f>B14*B6</f>
-        <v>302.93465958562501</v>
+        <v>322.46064719823704</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>35</v>
@@ -27577,7 +27578,7 @@
         <v>97</v>
       </c>
       <c r="J19" s="19">
-        <v>18.93</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>0</v>
@@ -27592,7 +27593,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="65">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>291</v>
@@ -27602,21 +27603,21 @@
       </c>
       <c r="J20" s="19">
         <f>J19*'Electric Motor'!D13</f>
-        <v>9843.6</v>
+        <v>10088</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L20" s="19">
         <f>J20/60</f>
-        <v>164.06</v>
+        <v>168.13333333333333</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>139</v>
       </c>
       <c r="N20" s="19">
         <f>J20*2*PI()/60</f>
-        <v>1030.8193814958829</v>
+        <v>1056.4128896471277</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>51</v>
@@ -27628,14 +27629,14 @@
       </c>
       <c r="B21" s="62">
         <f>B6/(B20*D19)</f>
-        <v>164.04199475065619</v>
+        <v>168.04301901286732</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="16">
         <f>B21*60</f>
-        <v>9842.5196850393713</v>
+        <v>10082.581140772039</v>
       </c>
       <c r="E21" t="s">
         <v>50</v>
@@ -27645,14 +27646,14 @@
       </c>
       <c r="J21" s="20">
         <f>J17*'weight analysis'!C4*L20^2*D19^4</f>
-        <v>31.303582231169969</v>
+        <v>32.877309565513919</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="20">
         <f>J21*0.224809</f>
-        <v>7.0373270178070895</v>
+        <v>7.3911150861136186</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>70</v>
@@ -27665,7 +27666,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="65">
-        <v>6.3E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>53</v>
@@ -27675,7 +27676,7 @@
       </c>
       <c r="J22" s="20">
         <f>J21/'weight analysis'!C25</f>
-        <v>0.23601618773557423</v>
+        <v>0.23910109804611884</v>
       </c>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
@@ -27689,7 +27690,7 @@
       </c>
       <c r="B23" s="64">
         <f>B22*B21^2*D19^4</f>
-        <v>14.632228799999998</v>
+        <v>16.085876753361095</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>55</v>
@@ -27699,7 +27700,7 @@
       </c>
       <c r="J23" s="20">
         <f>J18*'weight analysis'!C4*L20^3*D19^5</f>
-        <v>853.82776670060866</v>
+        <v>919.0171627616038</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>8</v>
@@ -27714,7 +27715,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="66">
-        <v>0.04</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>53</v>
@@ -27724,7 +27725,7 @@
       </c>
       <c r="J24" s="20">
         <f>J23/N20</f>
-        <v>0.82830007082479251</v>
+        <v>0.86994126233028257</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>9</v>
@@ -27740,7 +27741,7 @@
       </c>
       <c r="B25" s="65">
         <f>B22*B20/B24</f>
-        <v>0.66149999999999998</v>
+        <v>0.73135135135135143</v>
       </c>
       <c r="C25" s="19"/>
       <c r="I25" s="21" t="s">
@@ -27748,7 +27749,7 @@
       </c>
       <c r="J25" s="60">
         <f>J24/'Electric Motor'!F14+'Electric Motor'!D16</f>
-        <v>46.604477902831938</v>
+        <v>48.872018699051743</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>100</v>
@@ -27764,7 +27765,7 @@
       </c>
       <c r="B26" s="62">
         <f>B24*B21^3*D19^5</f>
-        <v>464.51519999999994</v>
+        <v>461.88936575615554</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>35</v>
@@ -27787,7 +27788,7 @@
       </c>
       <c r="B27" s="62">
         <f>B26/(2*PI()*B21)</f>
-        <v>0.45067661078916893</v>
+        <v>0.43745926580885602</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>61</v>
@@ -27797,7 +27798,7 @@
       </c>
       <c r="J27" s="24">
         <f>J23*J26</f>
-        <v>256148.3300101826</v>
+        <v>275705.14882848115</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>46</v>
@@ -27811,14 +27812,14 @@
       </c>
       <c r="J28" s="25">
         <f>J27/'weight analysis'!C17</f>
-        <v>4.2057111128211613</v>
+        <v>4.4333263740111288</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="20">
         <f>J28*0.224809</f>
-        <v>0.94548170956221245</v>
+        <v>0.99665166881506795</v>
       </c>
       <c r="M28" s="19" t="s">
         <v>70</v>
@@ -27897,7 +27898,7 @@
       </c>
       <c r="B8" s="62">
         <f>B6*'weight analysis'!C33/'weight analysis'!C3</f>
-        <v>484279.81215935299</v>
+        <v>441296.23640764045</v>
       </c>
       <c r="C8" s="19"/>
     </row>
@@ -27907,7 +27908,7 @@
       </c>
       <c r="B9" s="63">
         <f>'weight analysis'!C25/(B7*'weight analysis'!C31)</f>
-        <v>0.79791087047063713</v>
+        <v>0.99620591876672393</v>
       </c>
       <c r="C9" s="19"/>
     </row>
@@ -27926,7 +27927,7 @@
       </c>
       <c r="B11" s="63">
         <f>B9^2/(PI()*B10*'weight analysis'!C8)</f>
-        <v>4.3782429510822833E-2</v>
+        <v>6.8247905705751274E-2</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>104</v>
@@ -27950,7 +27951,7 @@
       </c>
       <c r="B13" s="63">
         <f>B12+B11</f>
-        <v>7.1882429510822826E-2</v>
+        <v>9.6347905705751274E-2</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>290</v>
@@ -27962,14 +27963,14 @@
       </c>
       <c r="B14" s="64">
         <f>B7*B13*'weight analysis'!C31</f>
-        <v>11.948698786584227</v>
+        <v>13.298659350451764</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D14">
         <f>B14/2</f>
-        <v>5.9743493932921137</v>
+        <v>6.6493296752258821</v>
       </c>
       <c r="E14" t="s">
         <v>279</v>
@@ -27981,7 +27982,7 @@
       </c>
       <c r="B15" s="62">
         <f>'weight analysis'!C25/B14</f>
-        <v>11.100221234877731</v>
+        <v>10.33967382549196</v>
       </c>
       <c r="C15" s="19"/>
     </row>
@@ -27991,7 +27992,7 @@
       </c>
       <c r="B16" s="20">
         <f>B14*B6</f>
-        <v>250.92267451826876</v>
+        <v>279.27184635948703</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>35</v>
@@ -28057,7 +28058,7 @@
         <v>97</v>
       </c>
       <c r="J19" s="19">
-        <v>18.07</v>
+        <v>18.75</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>0</v>
@@ -28072,7 +28073,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="65">
-        <v>0.44</v>
+        <v>0.42499999999999999</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>291</v>
@@ -28082,21 +28083,21 @@
       </c>
       <c r="J20" s="19">
         <f>J19*'Electric Motor'!D13</f>
-        <v>9396.4</v>
+        <v>9750</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>50</v>
       </c>
       <c r="L20" s="19">
         <f>J20/60</f>
-        <v>156.60666666666665</v>
+        <v>162.5</v>
       </c>
       <c r="M20" s="19" t="s">
         <v>139</v>
       </c>
       <c r="N20" s="19">
         <f>J20*2*PI()/60</f>
-        <v>983.98870700637099</v>
+        <v>1021.0176124166828</v>
       </c>
       <c r="O20" s="19" t="s">
         <v>51</v>
@@ -28108,14 +28109,14 @@
       </c>
       <c r="B21" s="62">
         <f>B6/(B20*D19)</f>
-        <v>156.58554044380818</v>
+        <v>162.11208893006022</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="16">
         <f>B21*60</f>
-        <v>9395.1324266284919</v>
+        <v>9726.7253358036141</v>
       </c>
       <c r="E21" t="s">
         <v>50</v>
@@ -28125,14 +28126,14 @@
       </c>
       <c r="J21" s="20">
         <f>J17*'weight analysis'!C4*L20^2*D19^4</f>
-        <v>27.745988930856502</v>
+        <v>29.873523377556321</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="20">
         <f>J21*0.224809</f>
-        <v>6.2375480255569196</v>
+        <v>6.7158369169850589</v>
       </c>
       <c r="M21" s="19" t="s">
         <v>70</v>
@@ -28145,7 +28146,7 @@
         <v>52</v>
       </c>
       <c r="B22" s="65">
-        <v>0.06</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>53</v>
@@ -28155,7 +28156,7 @@
       </c>
       <c r="J22" s="20">
         <f>J21/'weight analysis'!C25</f>
-        <v>0.20919339148008567</v>
+        <v>0.21725598403503263</v>
       </c>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
@@ -28169,7 +28170,7 @@
       </c>
       <c r="B23" s="64">
         <f>B22*B21^2*D19^4</f>
-        <v>12.697388628099173</v>
+        <v>13.836316562159165</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>55</v>
@@ -28179,7 +28180,7 @@
       </c>
       <c r="J23" s="20">
         <f>J18*'weight analysis'!C4*L20^3*D19^5</f>
-        <v>542.14536599433927</v>
+        <v>605.68261537007436</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>8</v>
@@ -28204,7 +28205,7 @@
       </c>
       <c r="J24" s="20">
         <f>J23/N20</f>
-        <v>0.55096706103846482</v>
+        <v>0.59321465957522779</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>9</v>
@@ -28220,7 +28221,7 @@
       </c>
       <c r="B25" s="65">
         <f>B22*B20/B24</f>
-        <v>0.69473684210526321</v>
+        <v>0.68223684210526314</v>
       </c>
       <c r="C25" s="19"/>
       <c r="I25" s="21" t="s">
@@ -28228,7 +28229,7 @@
       </c>
       <c r="J25" s="60">
         <f>J24/'Electric Motor'!F14+'Electric Motor'!D16</f>
-        <v>31.502510569692269</v>
+        <v>33.803072819737295</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>100</v>
@@ -28244,7 +28245,7 @@
       </c>
       <c r="B26" s="62">
         <f>B24*B21^3*D19^5</f>
-        <v>383.80742898572504</v>
+        <v>425.89703439163014</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>35</v>
@@ -28267,7 +28268,7 @@
       </c>
       <c r="B27" s="62">
         <f>B26/(2*PI()*B21)</f>
-        <v>0.39010530183909581</v>
+        <v>0.41812809099542647</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>61</v>
@@ -28277,7 +28278,7 @@
       </c>
       <c r="J27" s="24">
         <f>J23*J26</f>
-        <v>97586.165878981075</v>
+        <v>109022.87076661339</v>
       </c>
       <c r="K27" s="21" t="s">
         <v>46</v>
@@ -28291,14 +28292,14 @@
       </c>
       <c r="J28" s="25">
         <f>J27/'weight analysis'!C17</f>
-        <v>1.6022717082657718</v>
+        <v>1.7530828509870189</v>
       </c>
       <c r="K28" s="21" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="20">
         <f>J28*0.224809</f>
-        <v>0.36020510046351989</v>
+        <v>0.39410880264754072</v>
       </c>
       <c r="M28" s="19" t="s">
         <v>70</v>
@@ -28393,7 +28394,7 @@
       </c>
       <c r="N11" s="11">
         <f>PropWGlider!D21/'Electric Motor'!D13+'Electric Motor'!D16*'Electric Motor'!D19</f>
-        <v>19.032922471229561</v>
+        <v>19.494579116869307</v>
       </c>
       <c r="O11" t="s">
         <v>98</v>
@@ -28443,7 +28444,7 @@
       </c>
       <c r="N13" s="11">
         <f>PropWGlider!B27/'Electric Motor'!F14+'Electric Motor'!D16</f>
-        <v>26.041267046399991</v>
+        <v>25.321526138971368</v>
       </c>
       <c r="O13" t="s">
         <v>100</v>
@@ -28549,14 +28550,14 @@
       </c>
       <c r="N16" s="11">
         <f>((N13-'Electric Motor'!D16)*(N11-'Electric Motor'!D16*'Electric Motor'!D19))/(N11*N13)</f>
-        <v>0.93720012957952115</v>
+        <v>0.93569481494380236</v>
       </c>
       <c r="S16" s="21" t="s">
         <v>140</v>
       </c>
       <c r="T16" s="20">
         <f>T15/'weight analysis'!C25</f>
-        <v>0.11803581913666306</v>
+        <v>0.11385480551604289</v>
       </c>
       <c r="U16" s="19"/>
       <c r="V16" s="19"/>
@@ -28645,14 +28646,14 @@
       </c>
       <c r="T22" s="25">
         <f>T21/'weight analysis'!C17</f>
-        <v>6.6996403198619575E-2</v>
+        <v>6.561277502392375E-2</v>
       </c>
       <c r="U22" s="21" t="s">
         <v>9</v>
       </c>
       <c r="V22" s="20">
         <f>T22*0.224809</f>
-        <v>1.5061394406678469E-2</v>
+        <v>1.4750342340353275E-2</v>
       </c>
       <c r="W22" s="19" t="s">
         <v>70</v>

</xml_diff>